<commit_message>
Lagt till Iterationsplan för Iteration 1
</commit_message>
<xml_diff>
--- a/Iterationsplan_as223jx.xlsx
+++ b/Iterationsplan_as223jx.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="43" uniqueCount="29">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="75" uniqueCount="44">
   <si>
     <t>Tidsrapport v 14</t>
   </si>
@@ -103,6 +103,51 @@
   </si>
   <si>
     <t>Bestämde mig ganska snabbt att börja använda Eclipse.</t>
+  </si>
+  <si>
+    <t>Valde att försöka sätta mig in i Eclipse lite innan jag fortsätter med prototypen.</t>
+  </si>
+  <si>
+    <t>Tid sedan föregående iteration</t>
+  </si>
+  <si>
+    <t>Iterationsplan Iteration 1</t>
+  </si>
+  <si>
+    <t>Målet med denna iteration är att skapa en enkelt testapplikation genom att följa en stegvis beskrivning. Jag vill även kunna få Eclipse att fungera tillsammans med min Android-mobil vilket jag inte lyckats med ännu, så jag ska se om det är möjligt.</t>
+  </si>
+  <si>
+    <t>Handledarmöte</t>
+  </si>
+  <si>
+    <t>Ej påbörjad</t>
+  </si>
+  <si>
+    <t>Finslipning av vision</t>
+  </si>
+  <si>
+    <t>Påbörja testspecifikation och testfall</t>
+  </si>
+  <si>
+    <t>Systemtest och testrapport</t>
+  </si>
+  <si>
+    <t>Fortsätta arbeta med testapplikationen</t>
+  </si>
+  <si>
+    <t>Skapa iterationsplan för Iteration 2</t>
+  </si>
+  <si>
+    <t>Försöka få Eclipse att fungera med min mobil</t>
+  </si>
+  <si>
+    <t>Analys av föregående iteration</t>
+  </si>
+  <si>
+    <t>Har skapat en "Hello World"-app och med många om och men lyckats få en emulator att fungera som jag kan köra appen i. Försökte få det att fungera med min egen mobil men efter många försök så bestämde jag mig att köra emulator tills vidare. Fokuserade mest på att börja lära mig grunderna i Eclipse före att designa prototypen.</t>
+  </si>
+  <si>
+    <t>Iterationsplan as223jx</t>
   </si>
 </sst>
 </file>
@@ -126,7 +171,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="4">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -145,6 +190,12 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0" tint="-0.34998626667073579"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="1">
     <border>
@@ -158,7 +209,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -169,6 +220,9 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -472,21 +526,26 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A3:E27"/>
+  <dimension ref="A1:E50"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
-      <selection activeCell="E17" sqref="E17"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A3" sqref="A3:E3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="45.140625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="14.85546875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="28.85546875" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="10.7109375" customWidth="1"/>
     <col min="4" max="4" width="10.140625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="50.7109375" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="70.140625" customWidth="1"/>
   </cols>
   <sheetData>
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>43</v>
+      </c>
+    </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" s="5" t="s">
         <v>9</v>
@@ -494,6 +553,7 @@
       <c r="B3" s="5"/>
       <c r="C3" s="5"/>
       <c r="D3" s="5"/>
+      <c r="E3" s="5"/>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4" s="4" t="s">
@@ -502,6 +562,7 @@
       <c r="B4" s="4"/>
       <c r="C4" s="4"/>
       <c r="D4" s="4"/>
+      <c r="E4" s="4"/>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5" s="2" t="s">
@@ -581,8 +642,9 @@
       <c r="B13" s="4"/>
       <c r="C13" s="4"/>
       <c r="D13" s="4"/>
-    </row>
-    <row r="14" spans="1:5" ht="47.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="E13" s="4"/>
+    </row>
+    <row r="14" spans="1:5" ht="35.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A14" s="3" t="s">
         <v>21</v>
       </c>
@@ -612,9 +674,12 @@
         <v>12</v>
       </c>
       <c r="B17" t="s">
-        <v>26</v>
+        <v>23</v>
       </c>
       <c r="C17">
+        <v>1</v>
+      </c>
+      <c r="D17">
         <v>1</v>
       </c>
     </row>
@@ -623,10 +688,13 @@
         <v>13</v>
       </c>
       <c r="B18" t="s">
-        <v>26</v>
+        <v>23</v>
       </c>
       <c r="C18">
         <v>2</v>
+      </c>
+      <c r="D18">
+        <v>1</v>
       </c>
     </row>
     <row r="19" spans="1:5" x14ac:dyDescent="0.25">
@@ -662,7 +730,7 @@
         <v>14</v>
       </c>
       <c r="B21" t="s">
-        <v>26</v>
+        <v>23</v>
       </c>
       <c r="C21">
         <v>3</v>
@@ -679,13 +747,13 @@
         <v>15</v>
       </c>
       <c r="B22" t="s">
-        <v>26</v>
+        <v>11</v>
       </c>
       <c r="C22">
         <v>2</v>
       </c>
       <c r="D22">
-        <v>2</v>
+        <v>4</v>
       </c>
     </row>
     <row r="23" spans="1:5" x14ac:dyDescent="0.25">
@@ -698,15 +766,24 @@
       <c r="C23">
         <v>2</v>
       </c>
+      <c r="D23">
+        <v>0</v>
+      </c>
+      <c r="E23" t="s">
+        <v>29</v>
+      </c>
     </row>
     <row r="24" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
         <v>19</v>
       </c>
       <c r="B24" t="s">
-        <v>26</v>
+        <v>23</v>
       </c>
       <c r="C24">
+        <v>1</v>
+      </c>
+      <c r="D24">
         <v>1</v>
       </c>
     </row>
@@ -715,31 +792,225 @@
         <v>20</v>
       </c>
       <c r="B25" t="s">
-        <v>26</v>
+        <v>11</v>
       </c>
       <c r="C25">
         <v>2</v>
       </c>
-    </row>
-    <row r="26" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B26" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="C26">
-        <v>15</v>
+      <c r="D25">
+        <v>1</v>
       </c>
     </row>
     <row r="27" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B27" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="C27">
+        <v>15</v>
+      </c>
+      <c r="D27">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="28" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B28" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="D28">
+        <v>229</v>
+      </c>
+    </row>
+    <row r="29" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B29" s="1" t="s">
         <v>22</v>
       </c>
+      <c r="D29">
+        <v>240</v>
+      </c>
+    </row>
+    <row r="32" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A32" s="6" t="s">
+        <v>31</v>
+      </c>
+      <c r="B32" s="6"/>
+      <c r="C32" s="6"/>
+      <c r="D32" s="6"/>
+      <c r="E32" s="6"/>
+    </row>
+    <row r="33" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A33" s="4" t="s">
+        <v>41</v>
+      </c>
+      <c r="B33" s="4"/>
+      <c r="C33" s="4"/>
+      <c r="D33" s="4"/>
+      <c r="E33" s="4"/>
+    </row>
+    <row r="34" spans="1:5" ht="63" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A34" s="3" t="s">
+        <v>42</v>
+      </c>
+      <c r="B34" s="3"/>
+      <c r="C34" s="3"/>
+      <c r="D34" s="3"/>
+    </row>
+    <row r="35" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A35" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="B35" s="4"/>
+      <c r="C35" s="4"/>
+      <c r="D35" s="4"/>
+      <c r="E35" s="4"/>
+    </row>
+    <row r="36" spans="1:5" ht="48" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A36" s="3" t="s">
+        <v>32</v>
+      </c>
+      <c r="B36" s="3"/>
+      <c r="C36" s="3"/>
+      <c r="D36" s="3"/>
+    </row>
+    <row r="38" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A38" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="B38" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="C38" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="D38" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="E38" s="2" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="39" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A39" t="s">
+        <v>33</v>
+      </c>
+      <c r="B39" t="s">
+        <v>34</v>
+      </c>
+      <c r="C39">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="40" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A40" t="s">
+        <v>35</v>
+      </c>
+      <c r="B40" t="s">
+        <v>34</v>
+      </c>
+      <c r="C40">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="41" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A41" t="s">
+        <v>36</v>
+      </c>
+      <c r="B41" t="s">
+        <v>34</v>
+      </c>
+      <c r="C41">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="42" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A42" t="s">
+        <v>37</v>
+      </c>
+      <c r="B42" t="s">
+        <v>34</v>
+      </c>
+      <c r="C42">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="43" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A43" t="s">
+        <v>38</v>
+      </c>
+      <c r="B43" t="s">
+        <v>34</v>
+      </c>
+      <c r="C43">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="44" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A44" t="s">
+        <v>18</v>
+      </c>
+      <c r="B44" t="s">
+        <v>34</v>
+      </c>
+      <c r="C44">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="45" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A45" t="s">
+        <v>39</v>
+      </c>
+      <c r="B45" t="s">
+        <v>34</v>
+      </c>
+      <c r="C45">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="46" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A46" t="s">
+        <v>40</v>
+      </c>
+      <c r="B46" t="s">
+        <v>34</v>
+      </c>
+      <c r="C46">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="48" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B48" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="C48">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="49" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B49" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="D49">
+        <v>229</v>
+      </c>
+    </row>
+    <row r="50" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B50" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="D50">
+        <v>240</v>
+      </c>
     </row>
   </sheetData>
-  <mergeCells count="4">
+  <mergeCells count="9">
+    <mergeCell ref="A36:D36"/>
+    <mergeCell ref="A34:D34"/>
+    <mergeCell ref="A35:E35"/>
+    <mergeCell ref="A33:E33"/>
     <mergeCell ref="A14:D14"/>
-    <mergeCell ref="A4:D4"/>
-    <mergeCell ref="A3:D3"/>
-    <mergeCell ref="A13:D13"/>
+    <mergeCell ref="A32:E32"/>
+    <mergeCell ref="A13:E13"/>
+    <mergeCell ref="A4:E4"/>
+    <mergeCell ref="A3:E3"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967293" verticalDpi="0" r:id="rId1"/>

</xml_diff>

<commit_message>
Lagt till Iterationsplan för Iteration 2
</commit_message>
<xml_diff>
--- a/Iterationsplan_as223jx.xlsx
+++ b/Iterationsplan_as223jx.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9302"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="480" yWindow="30" windowWidth="22995" windowHeight="10050" activeTab="1"/>
+    <workbookView xWindow="480" yWindow="30" windowWidth="22995" windowHeight="10050" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Iteration 0" sheetId="1" r:id="rId1"/>
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="81" uniqueCount="49">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="112" uniqueCount="59">
   <si>
     <t>Tidsrapport v 14</t>
   </si>
@@ -126,9 +126,6 @@
     <t>Finslipning av vision</t>
   </si>
   <si>
-    <t>Fortsätta arbeta med testapplikationen</t>
-  </si>
-  <si>
     <t>Skapa iterationsplan för Iteration 2</t>
   </si>
   <si>
@@ -163,6 +160,39 @@
   </si>
   <si>
     <t>Skriv blackboxtester</t>
+  </si>
+  <si>
+    <t>Fixa textruta och action bar på testapplikationen</t>
+  </si>
+  <si>
+    <t>Iterationsplan Iteration 2</t>
+  </si>
+  <si>
+    <t>Jobbat med prototyp och persona, samt börjat implementera textfält, knappar och action bar i min testapplikation</t>
+  </si>
+  <si>
+    <t>Målet med denna iteration är att börja implementera grundläggande funktioner i min egen applikation.</t>
+  </si>
+  <si>
+    <t>Skapa sökruta</t>
+  </si>
+  <si>
+    <t>Skapa nytt projekt i Eclipse för min app</t>
+  </si>
+  <si>
+    <t>Skapa "Nytt recept"-knapp som öppnar ny sida</t>
+  </si>
+  <si>
+    <t>Planera färgtema &amp; bakgrund</t>
+  </si>
+  <si>
+    <t>Designa ikon till appen</t>
+  </si>
+  <si>
+    <t>Skapa textfälten samt sparaknapp i "Nytt recept"-sidan</t>
+  </si>
+  <si>
+    <t>Skapa Iterationsplan för Iteration 3</t>
   </si>
 </sst>
 </file>
@@ -224,7 +254,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -241,6 +271,9 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -560,7 +593,7 @@
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
@@ -912,13 +945,13 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E22"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A10" sqref="A10"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D21" sqref="D21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="41.5703125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="44.7109375" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="28.85546875" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="10.42578125" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="10.140625" bestFit="1" customWidth="1"/>
@@ -936,7 +969,7 @@
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" s="5" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="B2" s="5"/>
       <c r="C2" s="5"/>
@@ -945,7 +978,7 @@
     </row>
     <row r="3" spans="1:5" ht="63" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="7" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="B3" s="7"/>
       <c r="C3" s="7"/>
@@ -1001,7 +1034,7 @@
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="B9" t="s">
         <v>23</v>
@@ -1029,7 +1062,7 @@
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="B11" t="s">
         <v>23</v>
@@ -1043,7 +1076,7 @@
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="B12" t="s">
         <v>23</v>
@@ -1057,7 +1090,7 @@
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="B13" t="s">
         <v>34</v>
@@ -1065,24 +1098,27 @@
       <c r="C13">
         <v>1</v>
       </c>
+      <c r="D13">
+        <v>0</v>
+      </c>
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>36</v>
+        <v>48</v>
       </c>
       <c r="B14" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="C14">
         <v>4</v>
       </c>
       <c r="D14">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="B15" t="s">
         <v>23</v>
@@ -1096,7 +1132,7 @@
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="B16" t="s">
         <v>23</v>
@@ -1110,7 +1146,7 @@
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="B17" t="s">
         <v>34</v>
@@ -1118,16 +1154,22 @@
       <c r="C17">
         <v>1</v>
       </c>
+      <c r="D17">
+        <v>1</v>
+      </c>
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="B18" t="s">
         <v>34</v>
       </c>
       <c r="C18">
         <v>2</v>
+      </c>
+      <c r="D18">
+        <v>1</v>
       </c>
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.25">
@@ -1137,13 +1179,16 @@
       <c r="C20">
         <v>16</v>
       </c>
+      <c r="D20">
+        <v>13</v>
+      </c>
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B21" s="1" t="s">
         <v>30</v>
       </c>
       <c r="D21">
-        <v>229</v>
+        <v>216</v>
       </c>
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.25">
@@ -1168,12 +1213,213 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
+  <dimension ref="A1:E19"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D20" sqref="D20"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData/>
+  <cols>
+    <col min="1" max="1" width="50.7109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="28.85546875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="10.42578125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="10.140625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="11.42578125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A1" s="8" t="s">
+        <v>49</v>
+      </c>
+      <c r="B1" s="8"/>
+      <c r="C1" s="8"/>
+      <c r="D1" s="8"/>
+      <c r="E1" s="8"/>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A2" s="5" t="s">
+        <v>38</v>
+      </c>
+      <c r="B2" s="5"/>
+      <c r="C2" s="5"/>
+      <c r="D2" s="5"/>
+      <c r="E2" s="5"/>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A3" s="9" t="s">
+        <v>50</v>
+      </c>
+      <c r="B3" s="9"/>
+      <c r="C3" s="9"/>
+      <c r="D3" s="9"/>
+      <c r="E3" s="9"/>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A4" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="B4" s="5"/>
+      <c r="C4" s="5"/>
+      <c r="D4" s="5"/>
+      <c r="E4" s="5"/>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A5" s="7" t="s">
+        <v>51</v>
+      </c>
+      <c r="B5" s="7"/>
+      <c r="C5" s="7"/>
+      <c r="D5" s="7"/>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A7" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="B7" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="C7" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="D7" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="E7" s="2" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>33</v>
+      </c>
+      <c r="B8" t="s">
+        <v>34</v>
+      </c>
+      <c r="C8">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>53</v>
+      </c>
+      <c r="B9" t="s">
+        <v>34</v>
+      </c>
+      <c r="C9">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>54</v>
+      </c>
+      <c r="B10" t="s">
+        <v>34</v>
+      </c>
+      <c r="C10">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>57</v>
+      </c>
+      <c r="B11" t="s">
+        <v>34</v>
+      </c>
+      <c r="C11">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>46</v>
+      </c>
+      <c r="B12" t="s">
+        <v>34</v>
+      </c>
+      <c r="C12">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>52</v>
+      </c>
+      <c r="B13" t="s">
+        <v>34</v>
+      </c>
+      <c r="C13">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
+        <v>55</v>
+      </c>
+      <c r="B14" t="s">
+        <v>34</v>
+      </c>
+      <c r="C14">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
+        <v>56</v>
+      </c>
+      <c r="B15" t="s">
+        <v>34</v>
+      </c>
+      <c r="C15">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
+        <v>58</v>
+      </c>
+      <c r="B16" t="s">
+        <v>34</v>
+      </c>
+      <c r="C16">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="17" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B17" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="C17">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="18" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B18" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="D18">
+        <v>216</v>
+      </c>
+    </row>
+    <row r="19" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B19" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="D19">
+        <v>240</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="5">
+    <mergeCell ref="A1:E1"/>
+    <mergeCell ref="A2:E2"/>
+    <mergeCell ref="A4:E4"/>
+    <mergeCell ref="A5:D5"/>
+    <mergeCell ref="A3:E3"/>
+  </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Lagt till Iterationsplan för Iteration 3
Även lagt till mina Illustratorprojekt
</commit_message>
<xml_diff>
--- a/Iterationsplan_as223jx.xlsx
+++ b/Iterationsplan_as223jx.xlsx
@@ -4,19 +4,20 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9302"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="480" yWindow="30" windowWidth="22995" windowHeight="10050" activeTab="2"/>
+    <workbookView xWindow="480" yWindow="30" windowWidth="22995" windowHeight="10050" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="Iteration 0" sheetId="1" r:id="rId1"/>
     <sheet name="Iteration 1" sheetId="2" r:id="rId2"/>
-    <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
+    <sheet name="Iteration 2" sheetId="3" r:id="rId3"/>
+    <sheet name="Iteration 3" sheetId="4" r:id="rId4"/>
   </sheets>
   <calcPr calcId="144525"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="121" uniqueCount="65">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="156" uniqueCount="74">
   <si>
     <t>Tidsrapport v 14</t>
   </si>
@@ -192,15 +193,9 @@
     <t>Skapa sökruta på startsidan</t>
   </si>
   <si>
-    <t>Gör så "Spara"-knappen skickar och visar fältens information till ny sida</t>
-  </si>
-  <si>
     <t>Krav</t>
   </si>
   <si>
-    <t>Gör en exempeldesign i Illustrator</t>
-  </si>
-  <si>
     <t>F1</t>
   </si>
   <si>
@@ -211,6 +206,39 @@
   </si>
   <si>
     <t>F1/F2</t>
+  </si>
+  <si>
+    <t>Skapa dropdownlista för enheterna</t>
+  </si>
+  <si>
+    <t>Målet med denna Iteration är att jobba vidare med appen och förhoppningsvis bli klar med "Skapa recept"-sidan.</t>
+  </si>
+  <si>
+    <t>Göra klart dropdownen för enheter i Nytt Recept.</t>
+  </si>
+  <si>
+    <t>Skicka vidare infon från textfälten till ny "Visa Recept"-sida</t>
+  </si>
+  <si>
+    <t>Läs "Saving Data in SQL Databases" på Androids developersida.</t>
+  </si>
+  <si>
+    <t>Skapa Iterationsplan för Iteration 4</t>
+  </si>
+  <si>
+    <t>Gör en exempeldesign för startsidan i Illustrator</t>
+  </si>
+  <si>
+    <t>Gör exempeldesign för "Nytt recept"-sidan i Illustrator</t>
+  </si>
+  <si>
+    <t>Strukturera upp "Visa Recept"-sidan</t>
+  </si>
+  <si>
+    <t>Börjat jobba med min egen applikation. Insåg att dropdownlistan krånglade lite mer än jag förväntade mig, så det blir nog en del till tid för den.</t>
+  </si>
+  <si>
+    <t>F1-F4</t>
   </si>
 </sst>
 </file>
@@ -1233,8 +1261,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F20"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B11" sqref="B11"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="F14" sqref="F14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1244,7 +1272,7 @@
     <col min="3" max="3" width="28.85546875" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="10.42578125" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="10.140625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="11.42578125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="20.42578125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.25">
@@ -1299,7 +1327,7 @@
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A7" s="2" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="B7" s="2" t="s">
         <v>1</v>
@@ -1347,7 +1375,7 @@
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="B10" t="s">
         <v>53</v>
@@ -1364,7 +1392,7 @@
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="B11" t="s">
         <v>55</v>
@@ -1389,10 +1417,13 @@
       <c r="D12">
         <v>1</v>
       </c>
+      <c r="E12">
+        <v>0</v>
+      </c>
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="B13" t="s">
         <v>57</v>
@@ -1403,81 +1434,99 @@
       <c r="D13">
         <v>1</v>
       </c>
+      <c r="E13">
+        <v>0</v>
+      </c>
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="B14" t="s">
-        <v>60</v>
+        <v>69</v>
       </c>
       <c r="C14" t="s">
-        <v>43</v>
+        <v>23</v>
       </c>
       <c r="D14">
         <v>2</v>
       </c>
       <c r="E14">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="B15" t="s">
         <v>54</v>
       </c>
       <c r="C15" t="s">
-        <v>34</v>
+        <v>23</v>
       </c>
       <c r="D15">
+        <v>1</v>
+      </c>
+      <c r="E15">
         <v>1</v>
       </c>
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="B16" t="s">
-        <v>58</v>
+        <v>63</v>
       </c>
       <c r="C16" t="s">
-        <v>34</v>
+        <v>43</v>
       </c>
       <c r="D16">
         <v>2</v>
       </c>
-    </row>
-    <row r="17" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="E16">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="17" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B17" t="s">
         <v>56</v>
       </c>
       <c r="C17" t="s">
-        <v>34</v>
+        <v>23</v>
       </c>
       <c r="D17">
         <v>1</v>
       </c>
-    </row>
-    <row r="18" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="E17">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="18" spans="2:5" x14ac:dyDescent="0.25">
       <c r="C18" s="1" t="s">
         <v>6</v>
       </c>
       <c r="D18">
         <v>13</v>
       </c>
-    </row>
-    <row r="19" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="E18">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="19" spans="2:5" x14ac:dyDescent="0.25">
       <c r="C19" s="1" t="s">
         <v>30</v>
       </c>
-    </row>
-    <row r="20" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="E19">
+        <v>204</v>
+      </c>
+    </row>
+    <row r="20" spans="2:5" x14ac:dyDescent="0.25">
       <c r="C20" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="D20">
+      <c r="E20">
         <v>240</v>
       </c>
     </row>
@@ -1492,4 +1541,228 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967293" verticalDpi="0" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:F18"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A15" sqref="A15"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="5.85546875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="57.5703125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="28.85546875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="10.42578125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="10.140625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="16.5703125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A1" s="8" t="s">
+        <v>49</v>
+      </c>
+      <c r="B1" s="8"/>
+      <c r="C1" s="8"/>
+      <c r="D1" s="8"/>
+      <c r="E1" s="8"/>
+      <c r="F1" s="8"/>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A2" s="5" t="s">
+        <v>38</v>
+      </c>
+      <c r="B2" s="5"/>
+      <c r="C2" s="5"/>
+      <c r="D2" s="5"/>
+      <c r="E2" s="5"/>
+      <c r="F2" s="5"/>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A3" s="7" t="s">
+        <v>72</v>
+      </c>
+      <c r="B3" s="7"/>
+      <c r="C3" s="7"/>
+      <c r="D3" s="7"/>
+      <c r="E3" s="7"/>
+      <c r="F3" s="7"/>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A4" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="B4" s="5"/>
+      <c r="C4" s="5"/>
+      <c r="D4" s="5"/>
+      <c r="E4" s="5"/>
+      <c r="F4" s="5"/>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A5" s="9" t="s">
+        <v>64</v>
+      </c>
+      <c r="B5" s="9"/>
+      <c r="C5" s="9"/>
+      <c r="D5" s="9"/>
+      <c r="E5" s="9"/>
+      <c r="F5" s="9"/>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A7" s="2" t="s">
+        <v>58</v>
+      </c>
+      <c r="B7" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="C7" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="D7" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="E7" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="F7" s="2" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B8" t="s">
+        <v>33</v>
+      </c>
+      <c r="C8" t="s">
+        <v>34</v>
+      </c>
+      <c r="D8">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>59</v>
+      </c>
+      <c r="B9" t="s">
+        <v>65</v>
+      </c>
+      <c r="C9" t="s">
+        <v>34</v>
+      </c>
+      <c r="D9">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>62</v>
+      </c>
+      <c r="B10" t="s">
+        <v>66</v>
+      </c>
+      <c r="C10" t="s">
+        <v>34</v>
+      </c>
+      <c r="D10">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>60</v>
+      </c>
+      <c r="B11" t="s">
+        <v>71</v>
+      </c>
+      <c r="C11" t="s">
+        <v>34</v>
+      </c>
+      <c r="D11">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>59</v>
+      </c>
+      <c r="B12" t="s">
+        <v>70</v>
+      </c>
+      <c r="C12" t="s">
+        <v>34</v>
+      </c>
+      <c r="D12">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>73</v>
+      </c>
+      <c r="B13" t="s">
+        <v>67</v>
+      </c>
+      <c r="C13" t="s">
+        <v>34</v>
+      </c>
+      <c r="D13">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B14" t="s">
+        <v>46</v>
+      </c>
+      <c r="C14" t="s">
+        <v>34</v>
+      </c>
+      <c r="D14">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B15" t="s">
+        <v>68</v>
+      </c>
+      <c r="C15" t="s">
+        <v>34</v>
+      </c>
+      <c r="D15">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="C16" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="D16">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="17" spans="3:5" x14ac:dyDescent="0.25">
+      <c r="C17" s="1" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="18" spans="3:5" x14ac:dyDescent="0.25">
+      <c r="C18" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="E18">
+        <v>240</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="5">
+    <mergeCell ref="A1:F1"/>
+    <mergeCell ref="A2:F2"/>
+    <mergeCell ref="A3:F3"/>
+    <mergeCell ref="A4:F4"/>
+    <mergeCell ref="A5:F5"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Lagt till Iterationsplan för Iteration 4
</commit_message>
<xml_diff>
--- a/Iterationsplan_as223jx.xlsx
+++ b/Iterationsplan_as223jx.xlsx
@@ -4,20 +4,21 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9302"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="480" yWindow="30" windowWidth="22995" windowHeight="10050" activeTab="3"/>
+    <workbookView xWindow="480" yWindow="30" windowWidth="22995" windowHeight="10050" activeTab="4"/>
   </bookViews>
   <sheets>
     <sheet name="Iteration 0" sheetId="1" r:id="rId1"/>
     <sheet name="Iteration 1" sheetId="2" r:id="rId2"/>
     <sheet name="Iteration 2" sheetId="3" r:id="rId3"/>
     <sheet name="Iteration 3" sheetId="4" r:id="rId4"/>
+    <sheet name="Sheet1" sheetId="5" r:id="rId5"/>
   </sheets>
   <calcPr calcId="144525"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="156" uniqueCount="74">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="203" uniqueCount="91">
   <si>
     <t>Tidsrapport v 14</t>
   </si>
@@ -239,6 +240,57 @@
   </si>
   <si>
     <t>F1-F4</t>
+  </si>
+  <si>
+    <t>Gör så plusknappen skapar ny rad för ytterligare ingrediens</t>
+  </si>
+  <si>
+    <t>Skapa klickbar länk till sparat recept som visar receptet</t>
+  </si>
+  <si>
+    <t>Fixa så spinnern i nya ingrediensraderna fungerar</t>
+  </si>
+  <si>
+    <t>Skapa Iterationsplan för Iteration 5</t>
+  </si>
+  <si>
+    <t>Iterationsplan Iteration 4</t>
+  </si>
+  <si>
+    <t>Iterationsplan Iteration 3</t>
+  </si>
+  <si>
+    <t>Fixat så nya ingrediensrader dyker upp när man klickar på pluset. Även löst en bugg med min spinner/dropdownlista, men den funkar ännu inte i de nya ingrediensraderna.</t>
+  </si>
+  <si>
+    <t>Målet med denna iteration är att kunna spara recepten lokalt och att kunna visa dem.</t>
+  </si>
+  <si>
+    <t>Fixa så man kan spara lokalt</t>
+  </si>
+  <si>
+    <t>Gör så nya ingrediensradernas info också skickas vidare och sparas</t>
+  </si>
+  <si>
+    <t>Gör så spinnerns värde skickar vidare och sparas</t>
+  </si>
+  <si>
+    <t>Gör så man kan redigera ett existerande recept</t>
+  </si>
+  <si>
+    <t>Tester och testrapport</t>
+  </si>
+  <si>
+    <t>Fixa så texterna "Ingrediens" och "Antal" hamnar under nya ingrediensrader</t>
+  </si>
+  <si>
+    <t>F4</t>
+  </si>
+  <si>
+    <t>BK3</t>
+  </si>
+  <si>
+    <t>Läs tutorial om att spara lokalt</t>
   </si>
 </sst>
 </file>
@@ -1545,10 +1597,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F18"/>
+  <dimension ref="A1:F19"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A15" sqref="A15"/>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:F1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1563,7 +1615,7 @@
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1" s="8" t="s">
-        <v>49</v>
+        <v>79</v>
       </c>
       <c r="B1" s="8"/>
       <c r="C1" s="8"/>
@@ -1636,9 +1688,12 @@
         <v>33</v>
       </c>
       <c r="C8" t="s">
-        <v>34</v>
+        <v>23</v>
       </c>
       <c r="D8">
+        <v>1</v>
+      </c>
+      <c r="E8">
         <v>1</v>
       </c>
     </row>
@@ -1650,10 +1705,13 @@
         <v>65</v>
       </c>
       <c r="C9" t="s">
-        <v>34</v>
+        <v>23</v>
       </c>
       <c r="D9">
         <v>2</v>
+      </c>
+      <c r="E9">
+        <v>3</v>
       </c>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.25">
@@ -1664,10 +1722,284 @@
         <v>66</v>
       </c>
       <c r="C10" t="s">
-        <v>34</v>
+        <v>43</v>
       </c>
       <c r="D10">
         <v>4</v>
+      </c>
+      <c r="E10">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>59</v>
+      </c>
+      <c r="B11" t="s">
+        <v>74</v>
+      </c>
+      <c r="C11" t="s">
+        <v>43</v>
+      </c>
+      <c r="D11">
+        <v>1</v>
+      </c>
+      <c r="E11">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>60</v>
+      </c>
+      <c r="B12" t="s">
+        <v>71</v>
+      </c>
+      <c r="C12" t="s">
+        <v>43</v>
+      </c>
+      <c r="D12">
+        <v>2</v>
+      </c>
+      <c r="E12">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>59</v>
+      </c>
+      <c r="B13" t="s">
+        <v>70</v>
+      </c>
+      <c r="C13" t="s">
+        <v>23</v>
+      </c>
+      <c r="D13">
+        <v>2</v>
+      </c>
+      <c r="E13">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
+        <v>73</v>
+      </c>
+      <c r="B14" t="s">
+        <v>67</v>
+      </c>
+      <c r="C14" t="s">
+        <v>23</v>
+      </c>
+      <c r="D14">
+        <v>1</v>
+      </c>
+      <c r="E14">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B15" t="s">
+        <v>46</v>
+      </c>
+      <c r="C15" t="s">
+        <v>34</v>
+      </c>
+      <c r="D15">
+        <v>1</v>
+      </c>
+      <c r="E15">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B16" t="s">
+        <v>68</v>
+      </c>
+      <c r="C16" t="s">
+        <v>34</v>
+      </c>
+      <c r="D16">
+        <v>1</v>
+      </c>
+      <c r="E16">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="17" spans="3:5" x14ac:dyDescent="0.25">
+      <c r="C17" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="D17">
+        <v>15</v>
+      </c>
+      <c r="E17">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="18" spans="3:5" x14ac:dyDescent="0.25">
+      <c r="C18" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="E18">
+        <v>189</v>
+      </c>
+    </row>
+    <row r="19" spans="3:5" x14ac:dyDescent="0.25">
+      <c r="C19" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="E19">
+        <v>240</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="5">
+    <mergeCell ref="A1:F1"/>
+    <mergeCell ref="A2:F2"/>
+    <mergeCell ref="A3:F3"/>
+    <mergeCell ref="A4:F4"/>
+    <mergeCell ref="A5:F5"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:F21"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F13" sqref="F13"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="5.85546875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="69.85546875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="28.85546875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="10.42578125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="10.140625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="11.42578125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A1" s="8" t="s">
+        <v>78</v>
+      </c>
+      <c r="B1" s="8"/>
+      <c r="C1" s="8"/>
+      <c r="D1" s="8"/>
+      <c r="E1" s="8"/>
+      <c r="F1" s="8"/>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A2" s="5" t="s">
+        <v>38</v>
+      </c>
+      <c r="B2" s="5"/>
+      <c r="C2" s="5"/>
+      <c r="D2" s="5"/>
+      <c r="E2" s="5"/>
+      <c r="F2" s="5"/>
+    </row>
+    <row r="3" spans="1:6" ht="31.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A3" s="7" t="s">
+        <v>80</v>
+      </c>
+      <c r="B3" s="7"/>
+      <c r="C3" s="7"/>
+      <c r="D3" s="7"/>
+      <c r="E3" s="7"/>
+      <c r="F3" s="7"/>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A4" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="B4" s="5"/>
+      <c r="C4" s="5"/>
+      <c r="D4" s="5"/>
+      <c r="E4" s="5"/>
+      <c r="F4" s="5"/>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A5" s="9" t="s">
+        <v>81</v>
+      </c>
+      <c r="B5" s="9"/>
+      <c r="C5" s="9"/>
+      <c r="D5" s="9"/>
+      <c r="E5" s="9"/>
+      <c r="F5" s="9"/>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A7" s="2" t="s">
+        <v>58</v>
+      </c>
+      <c r="B7" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="C7" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="D7" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="E7" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="F7" s="2" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B8" t="s">
+        <v>33</v>
+      </c>
+      <c r="C8" t="s">
+        <v>23</v>
+      </c>
+      <c r="D8">
+        <v>1</v>
+      </c>
+      <c r="E8">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>59</v>
+      </c>
+      <c r="B9" t="s">
+        <v>90</v>
+      </c>
+      <c r="C9" t="s">
+        <v>34</v>
+      </c>
+      <c r="D9">
+        <v>2</v>
+      </c>
+      <c r="E9">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>59</v>
+      </c>
+      <c r="B10" t="s">
+        <v>82</v>
+      </c>
+      <c r="C10" t="s">
+        <v>34</v>
+      </c>
+      <c r="D10">
+        <v>8</v>
+      </c>
+      <c r="E10">
+        <v>2</v>
       </c>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.25">
@@ -1675,13 +2007,16 @@
         <v>60</v>
       </c>
       <c r="B11" t="s">
-        <v>71</v>
+        <v>75</v>
       </c>
       <c r="C11" t="s">
         <v>34</v>
       </c>
       <c r="D11">
-        <v>2</v>
+        <v>4</v>
+      </c>
+      <c r="E11">
+        <v>1</v>
       </c>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.25">
@@ -1689,21 +2024,21 @@
         <v>59</v>
       </c>
       <c r="B12" t="s">
-        <v>70</v>
+        <v>76</v>
       </c>
       <c r="C12" t="s">
         <v>34</v>
       </c>
       <c r="D12">
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>73</v>
+        <v>59</v>
       </c>
       <c r="B13" t="s">
-        <v>67</v>
+        <v>84</v>
       </c>
       <c r="C13" t="s">
         <v>34</v>
@@ -1713,45 +2048,87 @@
       </c>
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
+        <v>59</v>
+      </c>
       <c r="B14" t="s">
-        <v>46</v>
+        <v>83</v>
       </c>
       <c r="C14" t="s">
         <v>34</v>
       </c>
       <c r="D14">
-        <v>1</v>
+        <v>4</v>
       </c>
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
+        <v>88</v>
+      </c>
       <c r="B15" t="s">
-        <v>68</v>
+        <v>85</v>
       </c>
       <c r="C15" t="s">
         <v>34</v>
       </c>
       <c r="D15">
-        <v>1</v>
+        <v>10</v>
       </c>
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="C16" s="1" t="s">
+      <c r="A16" t="s">
+        <v>89</v>
+      </c>
+      <c r="B16" t="s">
+        <v>87</v>
+      </c>
+      <c r="C16" t="s">
+        <v>34</v>
+      </c>
+      <c r="D16">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="17" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B17" t="s">
+        <v>86</v>
+      </c>
+      <c r="C17" t="s">
+        <v>34</v>
+      </c>
+      <c r="D17">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="18" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B18" t="s">
+        <v>77</v>
+      </c>
+      <c r="C18" t="s">
+        <v>34</v>
+      </c>
+      <c r="D18">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="19" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="C19" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="D16">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="17" spans="3:5" x14ac:dyDescent="0.25">
-      <c r="C17" s="1" t="s">
+      <c r="D19">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="20" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="C20" s="1" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="18" spans="3:5" x14ac:dyDescent="0.25">
-      <c r="C18" s="1" t="s">
+    <row r="21" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="C21" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="E18">
+      <c r="E21">
         <v>240</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Lagt till Iterationsplan för Iteration 5
</commit_message>
<xml_diff>
--- a/Iterationsplan_as223jx.xlsx
+++ b/Iterationsplan_as223jx.xlsx
@@ -11,14 +11,15 @@
     <sheet name="Iteration 1" sheetId="2" r:id="rId2"/>
     <sheet name="Iteration 2" sheetId="3" r:id="rId3"/>
     <sheet name="Iteration 3" sheetId="4" r:id="rId4"/>
-    <sheet name="Sheet1" sheetId="5" r:id="rId5"/>
+    <sheet name="Iteration 4" sheetId="5" r:id="rId5"/>
+    <sheet name="Iteration 5" sheetId="6" r:id="rId6"/>
   </sheets>
   <calcPr calcId="144525"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="203" uniqueCount="91">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="250" uniqueCount="105">
   <si>
     <t>Tidsrapport v 14</t>
   </si>
@@ -266,9 +267,6 @@
     <t>Målet med denna iteration är att kunna spara recepten lokalt och att kunna visa dem.</t>
   </si>
   <si>
-    <t>Fixa så man kan spara lokalt</t>
-  </si>
-  <si>
     <t>Gör så nya ingrediensradernas info också skickas vidare och sparas</t>
   </si>
   <si>
@@ -291,6 +289,51 @@
   </si>
   <si>
     <t>Läs tutorial om att spara lokalt</t>
+  </si>
+  <si>
+    <t>Fixa så man kan spara hela recepten lokalt</t>
+  </si>
+  <si>
+    <t>Gör så recepten kan läsas in från startsidan</t>
+  </si>
+  <si>
+    <t>Mejla förra veckans jobb</t>
+  </si>
+  <si>
+    <t>Gör så man kan radera ett recept</t>
+  </si>
+  <si>
+    <t>Fixa scrollbars när texten fyller ut mer än hela sidora</t>
+  </si>
+  <si>
+    <t>Fixa hur filnamnen ska utformas med mellanslag i receptets namn</t>
+  </si>
+  <si>
+    <t>Gör så det inte är möjligt att spara ett recept om namnet redan finns</t>
+  </si>
+  <si>
+    <t>Gör så receptnamnen på framsidan visas utan ".txt" samt med stor bokstav</t>
+  </si>
+  <si>
+    <t>Justera och testa maxbredd och höjd på alla fält</t>
+  </si>
+  <si>
+    <t>Gör så "Ingrediens" och "Antal"-texten visas under nya ingrediensraderna</t>
+  </si>
+  <si>
+    <t>F3</t>
+  </si>
+  <si>
+    <t>BK1</t>
+  </si>
+  <si>
+    <t>Kan nu spara recept, visa alla existerande recept i en lista, samt öppna receptet och få det utskrivet.</t>
+  </si>
+  <si>
+    <t>Målet med denna iteration är att bli klar med alla grundfunktionaliteter, dvs har jag kvar att fixa så det går att redigera och radera recept. Efter det ska jag börja fixa med småbuggar, användarvänlighet och testing.</t>
+  </si>
+  <si>
+    <t>Iterationsplan Iteration 5</t>
   </si>
 </sst>
 </file>
@@ -1868,10 +1911,10 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F21"/>
+  <dimension ref="A1:F22"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F13" sqref="F13"/>
+      <selection activeCell="E18" sqref="E18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1973,16 +2016,16 @@
         <v>59</v>
       </c>
       <c r="B9" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="C9" t="s">
-        <v>34</v>
+        <v>23</v>
       </c>
       <c r="D9">
         <v>2</v>
       </c>
       <c r="E9">
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.25">
@@ -1990,16 +2033,16 @@
         <v>59</v>
       </c>
       <c r="B10" t="s">
-        <v>82</v>
+        <v>90</v>
       </c>
       <c r="C10" t="s">
-        <v>34</v>
+        <v>23</v>
       </c>
       <c r="D10">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="E10">
-        <v>2</v>
+        <v>6</v>
       </c>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.25">
@@ -2007,30 +2050,33 @@
         <v>60</v>
       </c>
       <c r="B11" t="s">
-        <v>75</v>
+        <v>91</v>
       </c>
       <c r="C11" t="s">
-        <v>34</v>
+        <v>23</v>
       </c>
       <c r="D11">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="E11">
-        <v>1</v>
+        <v>6</v>
       </c>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="B12" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="C12" t="s">
-        <v>34</v>
+        <v>23</v>
       </c>
       <c r="D12">
-        <v>3</v>
+        <v>2</v>
+      </c>
+      <c r="E12">
+        <v>5</v>
       </c>
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.25">
@@ -2038,13 +2084,16 @@
         <v>59</v>
       </c>
       <c r="B13" t="s">
-        <v>84</v>
+        <v>76</v>
       </c>
       <c r="C13" t="s">
-        <v>34</v>
+        <v>23</v>
       </c>
       <c r="D13">
-        <v>2</v>
+        <v>3</v>
+      </c>
+      <c r="E13">
+        <v>4</v>
       </c>
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.25">
@@ -2055,10 +2104,317 @@
         <v>83</v>
       </c>
       <c r="C14" t="s">
+        <v>23</v>
+      </c>
+      <c r="D14">
+        <v>2</v>
+      </c>
+      <c r="E14">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
+        <v>59</v>
+      </c>
+      <c r="B15" t="s">
+        <v>82</v>
+      </c>
+      <c r="C15" t="s">
+        <v>23</v>
+      </c>
+      <c r="D15">
+        <v>4</v>
+      </c>
+      <c r="E15">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
+        <v>87</v>
+      </c>
+      <c r="B16" t="s">
+        <v>84</v>
+      </c>
+      <c r="C16" t="s">
+        <v>43</v>
+      </c>
+      <c r="D16">
+        <v>8</v>
+      </c>
+      <c r="E16">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A17" t="s">
+        <v>88</v>
+      </c>
+      <c r="B17" t="s">
+        <v>86</v>
+      </c>
+      <c r="C17" t="s">
+        <v>43</v>
+      </c>
+      <c r="D17">
+        <v>1</v>
+      </c>
+      <c r="E17">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B18" t="s">
+        <v>85</v>
+      </c>
+      <c r="C18" t="s">
         <v>34</v>
       </c>
+      <c r="D18">
+        <v>4</v>
+      </c>
+      <c r="E18">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B19" t="s">
+        <v>77</v>
+      </c>
+      <c r="C19" t="s">
+        <v>23</v>
+      </c>
+      <c r="D19">
+        <v>1</v>
+      </c>
+      <c r="E19">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="C20" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="D20">
+        <v>38</v>
+      </c>
+      <c r="E20">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="C21" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="E21">
+        <v>153</v>
+      </c>
+    </row>
+    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="C22" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="E22">
+        <v>240</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="5">
+    <mergeCell ref="A1:F1"/>
+    <mergeCell ref="A2:F2"/>
+    <mergeCell ref="A3:F3"/>
+    <mergeCell ref="A4:F4"/>
+    <mergeCell ref="A5:F5"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:F22"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B20" sqref="B20"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="4.85546875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="69.85546875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="28.85546875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="10.42578125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="10.140625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="11.42578125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A1" s="8" t="s">
+        <v>104</v>
+      </c>
+      <c r="B1" s="8"/>
+      <c r="C1" s="8"/>
+      <c r="D1" s="8"/>
+      <c r="E1" s="8"/>
+      <c r="F1" s="8"/>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A2" s="5" t="s">
+        <v>38</v>
+      </c>
+      <c r="B2" s="5"/>
+      <c r="C2" s="5"/>
+      <c r="D2" s="5"/>
+      <c r="E2" s="5"/>
+      <c r="F2" s="5"/>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A3" s="7" t="s">
+        <v>102</v>
+      </c>
+      <c r="B3" s="7"/>
+      <c r="C3" s="7"/>
+      <c r="D3" s="7"/>
+      <c r="E3" s="7"/>
+      <c r="F3" s="7"/>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A4" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="B4" s="5"/>
+      <c r="C4" s="5"/>
+      <c r="D4" s="5"/>
+      <c r="E4" s="5"/>
+      <c r="F4" s="5"/>
+    </row>
+    <row r="5" spans="1:6" ht="31.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A5" s="9" t="s">
+        <v>103</v>
+      </c>
+      <c r="B5" s="9"/>
+      <c r="C5" s="9"/>
+      <c r="D5" s="9"/>
+      <c r="E5" s="9"/>
+      <c r="F5" s="9"/>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A7" s="2" t="s">
+        <v>58</v>
+      </c>
+      <c r="B7" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="C7" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="D7" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="E7" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="F7" s="2" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B8" t="s">
+        <v>92</v>
+      </c>
+      <c r="C8" t="s">
+        <v>23</v>
+      </c>
+      <c r="D8">
+        <v>1</v>
+      </c>
+      <c r="E8">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>87</v>
+      </c>
+      <c r="B9" t="s">
+        <v>84</v>
+      </c>
+      <c r="C9" t="s">
+        <v>34</v>
+      </c>
+      <c r="D9">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>100</v>
+      </c>
+      <c r="B10" t="s">
+        <v>93</v>
+      </c>
+      <c r="C10" t="s">
+        <v>34</v>
+      </c>
+      <c r="D10">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>101</v>
+      </c>
+      <c r="B11" t="s">
+        <v>98</v>
+      </c>
+      <c r="C11" t="s">
+        <v>34</v>
+      </c>
+      <c r="D11">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>101</v>
+      </c>
+      <c r="B12" t="s">
+        <v>94</v>
+      </c>
+      <c r="C12" t="s">
+        <v>34</v>
+      </c>
+      <c r="D12">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>59</v>
+      </c>
+      <c r="B13" t="s">
+        <v>95</v>
+      </c>
+      <c r="C13" t="s">
+        <v>34</v>
+      </c>
+      <c r="D13">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
+        <v>59</v>
+      </c>
+      <c r="B14" t="s">
+        <v>96</v>
+      </c>
+      <c r="C14" t="s">
+        <v>34</v>
+      </c>
       <c r="D14">
-        <v>4</v>
+        <v>2</v>
       </c>
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.25">
@@ -2066,69 +2422,69 @@
         <v>88</v>
       </c>
       <c r="B15" t="s">
-        <v>85</v>
+        <v>97</v>
       </c>
       <c r="C15" t="s">
         <v>34</v>
       </c>
       <c r="D15">
-        <v>10</v>
+        <v>3</v>
       </c>
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="B16" t="s">
-        <v>87</v>
+        <v>99</v>
       </c>
       <c r="C16" t="s">
-        <v>34</v>
+        <v>43</v>
       </c>
       <c r="D16">
-        <v>1</v>
+        <v>4</v>
       </c>
     </row>
     <row r="17" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B17" t="s">
-        <v>86</v>
+        <v>68</v>
       </c>
       <c r="C17" t="s">
-        <v>34</v>
+        <v>43</v>
       </c>
       <c r="D17">
-        <v>4</v>
+        <v>1</v>
       </c>
     </row>
     <row r="18" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B18" t="s">
-        <v>77</v>
+        <v>85</v>
       </c>
       <c r="C18" t="s">
-        <v>34</v>
+        <v>43</v>
       </c>
       <c r="D18">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="19" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="C19" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="D19">
-        <v>40</v>
+        <v>4</v>
       </c>
     </row>
     <row r="20" spans="2:5" x14ac:dyDescent="0.25">
       <c r="C20" s="1" t="s">
-        <v>30</v>
+        <v>6</v>
+      </c>
+      <c r="D20">
+        <v>40</v>
       </c>
     </row>
     <row r="21" spans="2:5" x14ac:dyDescent="0.25">
       <c r="C21" s="1" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="22" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="C22" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="E21">
+      <c r="E22">
         <v>240</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Lagt till Iterationsplan för Iteration 6
Även lagt till Testrapport
</commit_message>
<xml_diff>
--- a/Iterationsplan_as223jx.xlsx
+++ b/Iterationsplan_as223jx.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9302"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="480" yWindow="30" windowWidth="22995" windowHeight="10050" activeTab="5"/>
+    <workbookView xWindow="480" yWindow="30" windowWidth="22995" windowHeight="10050" activeTab="7"/>
   </bookViews>
   <sheets>
     <sheet name="Iteration 0" sheetId="1" r:id="rId1"/>
@@ -13,13 +13,15 @@
     <sheet name="Iteration 3" sheetId="4" r:id="rId4"/>
     <sheet name="Iteration 4" sheetId="5" r:id="rId5"/>
     <sheet name="Iteration 5" sheetId="6" r:id="rId6"/>
+    <sheet name="Iteration 6" sheetId="7" r:id="rId7"/>
+    <sheet name="Sheet2" sheetId="8" r:id="rId8"/>
   </sheets>
   <calcPr calcId="144525"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="250" uniqueCount="105">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="327" uniqueCount="129">
   <si>
     <t>Tidsrapport v 14</t>
   </si>
@@ -318,9 +320,6 @@
     <t>Justera och testa maxbredd och höjd på alla fält</t>
   </si>
   <si>
-    <t>Gör så "Ingrediens" och "Antal"-texten visas under nya ingrediensraderna</t>
-  </si>
-  <si>
     <t>F3</t>
   </si>
   <si>
@@ -334,6 +333,81 @@
   </si>
   <si>
     <t>Iterationsplan Iteration 5</t>
+  </si>
+  <si>
+    <t>Workshop</t>
+  </si>
+  <si>
+    <t>Skapa Iterationsplan för Iteration 6</t>
+  </si>
+  <si>
+    <t>Handledningsmöte</t>
+  </si>
+  <si>
+    <t>Gör klart så infon läggs rätt i Redigera Recept</t>
+  </si>
+  <si>
+    <t>Skapa Iterationsplan för Iteration 7</t>
+  </si>
+  <si>
+    <t>Iterationsplan Iteration 6</t>
+  </si>
+  <si>
+    <t>Fixa så spinnersen har rätt defaultvärde i Redigera Recept</t>
+  </si>
+  <si>
+    <t>Finslipa testspecifikationen</t>
+  </si>
+  <si>
+    <t>Lägg till "Redigera" och "Ta bort"-knappar i Visa Recept</t>
+  </si>
+  <si>
+    <t>F3/F4</t>
+  </si>
+  <si>
+    <t>Jobbat med att kunna redigera recept, delar ut infon från receptet i korrekta redigeringsbara textrutor.</t>
+  </si>
+  <si>
+    <t>Målet med denna iteration är att fixa klart så all info i Redigera Recept hamnar rätt, samt börja med hantering av inmatning, scrollbars, textfält.</t>
+  </si>
+  <si>
+    <t>Iterationsplan Iteration 7</t>
+  </si>
+  <si>
+    <t>Fortsatt (och fastnat) med att lägga ut infon i rätt rutor med rätt värden i Redigera Recept. Får inte till dropdown-rutorna.</t>
+  </si>
+  <si>
+    <t>Fixa så de nya aktiviteterna ej hamnar uppepå varandra vid radering.</t>
+  </si>
+  <si>
+    <t>Uppdatera MainActivity då ett nytt recept har skapats.</t>
+  </si>
+  <si>
+    <t>Testa navigera mellan alla olika aktiviteter och se till att inga problem finns kvar med detta.</t>
+  </si>
+  <si>
+    <t>Fixa att om man ändrar namn i Redigera Recept ska den gamla filen tas bort och en ny sparas med nya namnet.</t>
+  </si>
+  <si>
+    <t>Skapa Iterationsplan för Iteration 8</t>
+  </si>
+  <si>
+    <t>Fixa så nya receptradernas "Antal"-textfält har siffror som standardinmatning.</t>
+  </si>
+  <si>
+    <t>Fixa så receptet inte sparas om inte alla ingrediensrader är korrekt ifyllda.</t>
+  </si>
+  <si>
+    <t>Fixa så om man lämnar en receptrad helt tom ska det ändå gå att spara receptet. (Raden ignoreras)</t>
+  </si>
+  <si>
+    <t>Gör så det går att spara med samma namn som receptet som redigeras, men inte andra existerande receptnamn</t>
+  </si>
+  <si>
+    <t>Skapa bekräftelsepopupruta vid radering av recept.</t>
+  </si>
+  <si>
+    <t>Ändra grundfärgerna på knappar och bakgrund.</t>
   </si>
 </sst>
 </file>
@@ -395,12 +469,15 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -738,22 +815,22 @@
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A3" s="6" t="s">
+      <c r="A3" s="7" t="s">
         <v>9</v>
       </c>
-      <c r="B3" s="6"/>
-      <c r="C3" s="6"/>
-      <c r="D3" s="6"/>
-      <c r="E3" s="6"/>
+      <c r="B3" s="7"/>
+      <c r="C3" s="7"/>
+      <c r="D3" s="7"/>
+      <c r="E3" s="7"/>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A4" s="5" t="s">
+      <c r="A4" s="6" t="s">
         <v>0</v>
       </c>
-      <c r="B4" s="5"/>
-      <c r="C4" s="5"/>
-      <c r="D4" s="5"/>
-      <c r="E4" s="5"/>
+      <c r="B4" s="6"/>
+      <c r="C4" s="6"/>
+      <c r="D4" s="6"/>
+      <c r="E4" s="6"/>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5" s="2" t="s">
@@ -827,21 +904,21 @@
       </c>
     </row>
     <row r="13" spans="1:5" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A13" s="5" t="s">
+      <c r="A13" s="6" t="s">
         <v>7</v>
       </c>
-      <c r="B13" s="5"/>
-      <c r="C13" s="5"/>
-      <c r="D13" s="5"/>
-      <c r="E13" s="5"/>
+      <c r="B13" s="6"/>
+      <c r="C13" s="6"/>
+      <c r="D13" s="6"/>
+      <c r="E13" s="6"/>
     </row>
     <row r="14" spans="1:5" ht="35.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A14" s="7" t="s">
+      <c r="A14" s="8" t="s">
         <v>21</v>
       </c>
-      <c r="B14" s="7"/>
-      <c r="C14" s="7"/>
-      <c r="D14" s="7"/>
+      <c r="B14" s="8"/>
+      <c r="C14" s="8"/>
+      <c r="D14" s="8"/>
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A16" s="2" t="s">
@@ -1100,47 +1177,47 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A1" s="8" t="s">
+      <c r="A1" s="9" t="s">
         <v>31</v>
       </c>
-      <c r="B1" s="8"/>
-      <c r="C1" s="8"/>
-      <c r="D1" s="8"/>
-      <c r="E1" s="8"/>
+      <c r="B1" s="9"/>
+      <c r="C1" s="9"/>
+      <c r="D1" s="9"/>
+      <c r="E1" s="9"/>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A2" s="5" t="s">
+      <c r="A2" s="6" t="s">
         <v>38</v>
       </c>
-      <c r="B2" s="5"/>
-      <c r="C2" s="5"/>
-      <c r="D2" s="5"/>
-      <c r="E2" s="5"/>
+      <c r="B2" s="6"/>
+      <c r="C2" s="6"/>
+      <c r="D2" s="6"/>
+      <c r="E2" s="6"/>
     </row>
     <row r="3" spans="1:5" ht="63" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="7" t="s">
+      <c r="A3" s="8" t="s">
         <v>39</v>
       </c>
-      <c r="B3" s="7"/>
-      <c r="C3" s="7"/>
-      <c r="D3" s="7"/>
+      <c r="B3" s="8"/>
+      <c r="C3" s="8"/>
+      <c r="D3" s="8"/>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A4" s="5" t="s">
+      <c r="A4" s="6" t="s">
         <v>7</v>
       </c>
-      <c r="B4" s="5"/>
-      <c r="C4" s="5"/>
-      <c r="D4" s="5"/>
-      <c r="E4" s="5"/>
+      <c r="B4" s="6"/>
+      <c r="C4" s="6"/>
+      <c r="D4" s="6"/>
+      <c r="E4" s="6"/>
     </row>
     <row r="5" spans="1:5" ht="49.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="7" t="s">
+      <c r="A5" s="8" t="s">
         <v>32</v>
       </c>
-      <c r="B5" s="7"/>
-      <c r="C5" s="7"/>
-      <c r="D5" s="7"/>
+      <c r="B5" s="8"/>
+      <c r="C5" s="8"/>
+      <c r="D5" s="8"/>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A7" s="2" t="s">
@@ -1371,54 +1448,54 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A1" s="8" t="s">
+      <c r="A1" s="9" t="s">
         <v>49</v>
       </c>
-      <c r="B1" s="8"/>
-      <c r="C1" s="8"/>
-      <c r="D1" s="8"/>
-      <c r="E1" s="8"/>
-      <c r="F1" s="8"/>
+      <c r="B1" s="9"/>
+      <c r="C1" s="9"/>
+      <c r="D1" s="9"/>
+      <c r="E1" s="9"/>
+      <c r="F1" s="9"/>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A2" s="5" t="s">
+      <c r="A2" s="6" t="s">
         <v>38</v>
       </c>
-      <c r="B2" s="5"/>
-      <c r="C2" s="5"/>
-      <c r="D2" s="5"/>
-      <c r="E2" s="5"/>
-      <c r="F2" s="5"/>
+      <c r="B2" s="6"/>
+      <c r="C2" s="6"/>
+      <c r="D2" s="6"/>
+      <c r="E2" s="6"/>
+      <c r="F2" s="6"/>
     </row>
     <row r="3" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="7" t="s">
+      <c r="A3" s="8" t="s">
         <v>50</v>
       </c>
-      <c r="B3" s="7"/>
-      <c r="C3" s="7"/>
-      <c r="D3" s="7"/>
-      <c r="E3" s="7"/>
-      <c r="F3" s="7"/>
+      <c r="B3" s="8"/>
+      <c r="C3" s="8"/>
+      <c r="D3" s="8"/>
+      <c r="E3" s="8"/>
+      <c r="F3" s="8"/>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A4" s="5" t="s">
+      <c r="A4" s="6" t="s">
         <v>7</v>
       </c>
-      <c r="B4" s="5"/>
-      <c r="C4" s="5"/>
-      <c r="D4" s="5"/>
-      <c r="E4" s="5"/>
-      <c r="F4" s="5"/>
+      <c r="B4" s="6"/>
+      <c r="C4" s="6"/>
+      <c r="D4" s="6"/>
+      <c r="E4" s="6"/>
+      <c r="F4" s="6"/>
     </row>
     <row r="5" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="9" t="s">
+      <c r="A5" s="10" t="s">
         <v>51</v>
       </c>
-      <c r="B5" s="9"/>
-      <c r="C5" s="9"/>
-      <c r="D5" s="9"/>
-      <c r="E5" s="9"/>
-      <c r="F5" s="9"/>
+      <c r="B5" s="10"/>
+      <c r="C5" s="10"/>
+      <c r="D5" s="10"/>
+      <c r="E5" s="10"/>
+      <c r="F5" s="10"/>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A7" s="2" t="s">
@@ -1657,54 +1734,54 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A1" s="8" t="s">
+      <c r="A1" s="9" t="s">
         <v>79</v>
       </c>
-      <c r="B1" s="8"/>
-      <c r="C1" s="8"/>
-      <c r="D1" s="8"/>
-      <c r="E1" s="8"/>
-      <c r="F1" s="8"/>
+      <c r="B1" s="9"/>
+      <c r="C1" s="9"/>
+      <c r="D1" s="9"/>
+      <c r="E1" s="9"/>
+      <c r="F1" s="9"/>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A2" s="5" t="s">
+      <c r="A2" s="6" t="s">
         <v>38</v>
       </c>
-      <c r="B2" s="5"/>
-      <c r="C2" s="5"/>
-      <c r="D2" s="5"/>
-      <c r="E2" s="5"/>
-      <c r="F2" s="5"/>
+      <c r="B2" s="6"/>
+      <c r="C2" s="6"/>
+      <c r="D2" s="6"/>
+      <c r="E2" s="6"/>
+      <c r="F2" s="6"/>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A3" s="7" t="s">
+      <c r="A3" s="8" t="s">
         <v>72</v>
       </c>
-      <c r="B3" s="7"/>
-      <c r="C3" s="7"/>
-      <c r="D3" s="7"/>
-      <c r="E3" s="7"/>
-      <c r="F3" s="7"/>
+      <c r="B3" s="8"/>
+      <c r="C3" s="8"/>
+      <c r="D3" s="8"/>
+      <c r="E3" s="8"/>
+      <c r="F3" s="8"/>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A4" s="5" t="s">
+      <c r="A4" s="6" t="s">
         <v>7</v>
       </c>
-      <c r="B4" s="5"/>
-      <c r="C4" s="5"/>
-      <c r="D4" s="5"/>
-      <c r="E4" s="5"/>
-      <c r="F4" s="5"/>
+      <c r="B4" s="6"/>
+      <c r="C4" s="6"/>
+      <c r="D4" s="6"/>
+      <c r="E4" s="6"/>
+      <c r="F4" s="6"/>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A5" s="9" t="s">
+      <c r="A5" s="10" t="s">
         <v>64</v>
       </c>
-      <c r="B5" s="9"/>
-      <c r="C5" s="9"/>
-      <c r="D5" s="9"/>
-      <c r="E5" s="9"/>
-      <c r="F5" s="9"/>
+      <c r="B5" s="10"/>
+      <c r="C5" s="10"/>
+      <c r="D5" s="10"/>
+      <c r="E5" s="10"/>
+      <c r="F5" s="10"/>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A7" s="2" t="s">
@@ -1928,54 +2005,54 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A1" s="8" t="s">
+      <c r="A1" s="9" t="s">
         <v>78</v>
       </c>
-      <c r="B1" s="8"/>
-      <c r="C1" s="8"/>
-      <c r="D1" s="8"/>
-      <c r="E1" s="8"/>
-      <c r="F1" s="8"/>
+      <c r="B1" s="9"/>
+      <c r="C1" s="9"/>
+      <c r="D1" s="9"/>
+      <c r="E1" s="9"/>
+      <c r="F1" s="9"/>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A2" s="5" t="s">
+      <c r="A2" s="6" t="s">
         <v>38</v>
       </c>
-      <c r="B2" s="5"/>
-      <c r="C2" s="5"/>
-      <c r="D2" s="5"/>
-      <c r="E2" s="5"/>
-      <c r="F2" s="5"/>
+      <c r="B2" s="6"/>
+      <c r="C2" s="6"/>
+      <c r="D2" s="6"/>
+      <c r="E2" s="6"/>
+      <c r="F2" s="6"/>
     </row>
     <row r="3" spans="1:6" ht="31.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="7" t="s">
+      <c r="A3" s="8" t="s">
         <v>80</v>
       </c>
-      <c r="B3" s="7"/>
-      <c r="C3" s="7"/>
-      <c r="D3" s="7"/>
-      <c r="E3" s="7"/>
-      <c r="F3" s="7"/>
+      <c r="B3" s="8"/>
+      <c r="C3" s="8"/>
+      <c r="D3" s="8"/>
+      <c r="E3" s="8"/>
+      <c r="F3" s="8"/>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A4" s="5" t="s">
+      <c r="A4" s="6" t="s">
         <v>7</v>
       </c>
-      <c r="B4" s="5"/>
-      <c r="C4" s="5"/>
-      <c r="D4" s="5"/>
-      <c r="E4" s="5"/>
-      <c r="F4" s="5"/>
+      <c r="B4" s="6"/>
+      <c r="C4" s="6"/>
+      <c r="D4" s="6"/>
+      <c r="E4" s="6"/>
+      <c r="F4" s="6"/>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A5" s="9" t="s">
+      <c r="A5" s="10" t="s">
         <v>81</v>
       </c>
-      <c r="B5" s="9"/>
-      <c r="C5" s="9"/>
-      <c r="D5" s="9"/>
-      <c r="E5" s="9"/>
-      <c r="F5" s="9"/>
+      <c r="B5" s="10"/>
+      <c r="C5" s="10"/>
+      <c r="D5" s="10"/>
+      <c r="E5" s="10"/>
+      <c r="F5" s="10"/>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A7" s="2" t="s">
@@ -2235,8 +2312,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F22"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F17" sqref="F17"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C31" sqref="C31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2250,54 +2327,54 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A1" s="8" t="s">
-        <v>104</v>
-      </c>
-      <c r="B1" s="8"/>
-      <c r="C1" s="8"/>
-      <c r="D1" s="8"/>
-      <c r="E1" s="8"/>
-      <c r="F1" s="8"/>
+      <c r="A1" s="9" t="s">
+        <v>103</v>
+      </c>
+      <c r="B1" s="9"/>
+      <c r="C1" s="9"/>
+      <c r="D1" s="9"/>
+      <c r="E1" s="9"/>
+      <c r="F1" s="9"/>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A2" s="5" t="s">
+      <c r="A2" s="6" t="s">
         <v>38</v>
       </c>
-      <c r="B2" s="5"/>
-      <c r="C2" s="5"/>
-      <c r="D2" s="5"/>
-      <c r="E2" s="5"/>
-      <c r="F2" s="5"/>
+      <c r="B2" s="6"/>
+      <c r="C2" s="6"/>
+      <c r="D2" s="6"/>
+      <c r="E2" s="6"/>
+      <c r="F2" s="6"/>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A3" s="7" t="s">
+      <c r="A3" s="8" t="s">
+        <v>101</v>
+      </c>
+      <c r="B3" s="8"/>
+      <c r="C3" s="8"/>
+      <c r="D3" s="8"/>
+      <c r="E3" s="8"/>
+      <c r="F3" s="8"/>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A4" s="6" t="s">
+        <v>7</v>
+      </c>
+      <c r="B4" s="6"/>
+      <c r="C4" s="6"/>
+      <c r="D4" s="6"/>
+      <c r="E4" s="6"/>
+      <c r="F4" s="6"/>
+    </row>
+    <row r="5" spans="1:6" ht="31.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A5" s="10" t="s">
         <v>102</v>
       </c>
-      <c r="B3" s="7"/>
-      <c r="C3" s="7"/>
-      <c r="D3" s="7"/>
-      <c r="E3" s="7"/>
-      <c r="F3" s="7"/>
-    </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A4" s="5" t="s">
-        <v>7</v>
-      </c>
-      <c r="B4" s="5"/>
-      <c r="C4" s="5"/>
-      <c r="D4" s="5"/>
-      <c r="E4" s="5"/>
-      <c r="F4" s="5"/>
-    </row>
-    <row r="5" spans="1:6" ht="31.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="9" t="s">
-        <v>103</v>
-      </c>
-      <c r="B5" s="9"/>
-      <c r="C5" s="9"/>
-      <c r="D5" s="9"/>
-      <c r="E5" s="9"/>
-      <c r="F5" s="9"/>
+      <c r="B5" s="10"/>
+      <c r="C5" s="10"/>
+      <c r="D5" s="10"/>
+      <c r="E5" s="10"/>
+      <c r="F5" s="10"/>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A7" s="2" t="s">
@@ -2341,18 +2418,18 @@
         <v>84</v>
       </c>
       <c r="C9" t="s">
-        <v>34</v>
+        <v>43</v>
       </c>
       <c r="D9">
         <v>10</v>
       </c>
       <c r="E9">
-        <v>5</v>
+        <v>15</v>
       </c>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="B10" t="s">
         <v>93</v>
@@ -2363,24 +2440,30 @@
       <c r="D10">
         <v>5</v>
       </c>
+      <c r="E10">
+        <v>0</v>
+      </c>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="B11" t="s">
         <v>98</v>
       </c>
       <c r="C11" t="s">
-        <v>34</v>
+        <v>43</v>
       </c>
       <c r="D11">
         <v>4</v>
       </c>
+      <c r="E11">
+        <v>4</v>
+      </c>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="B12" t="s">
         <v>94</v>
@@ -2390,6 +2473,9 @@
       </c>
       <c r="D12">
         <v>3</v>
+      </c>
+      <c r="E12">
+        <v>0</v>
       </c>
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.25">
@@ -2400,9 +2486,12 @@
         <v>95</v>
       </c>
       <c r="C13" t="s">
-        <v>34</v>
+        <v>23</v>
       </c>
       <c r="D13">
+        <v>3</v>
+      </c>
+      <c r="E13">
         <v>3</v>
       </c>
     </row>
@@ -2414,9 +2503,12 @@
         <v>96</v>
       </c>
       <c r="C14" t="s">
-        <v>34</v>
+        <v>23</v>
       </c>
       <c r="D14">
+        <v>2</v>
+      </c>
+      <c r="E14">
         <v>2</v>
       </c>
     </row>
@@ -2428,34 +2520,40 @@
         <v>97</v>
       </c>
       <c r="C15" t="s">
-        <v>34</v>
+        <v>23</v>
       </c>
       <c r="D15">
         <v>3</v>
       </c>
+      <c r="E15">
+        <v>3</v>
+      </c>
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A16" t="s">
-        <v>88</v>
-      </c>
       <c r="B16" t="s">
-        <v>99</v>
+        <v>104</v>
       </c>
       <c r="C16" t="s">
-        <v>43</v>
+        <v>23</v>
       </c>
       <c r="D16">
-        <v>4</v>
+        <v>3</v>
+      </c>
+      <c r="E16">
+        <v>3</v>
       </c>
     </row>
     <row r="17" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B17" t="s">
-        <v>68</v>
+        <v>105</v>
       </c>
       <c r="C17" t="s">
-        <v>43</v>
+        <v>34</v>
       </c>
       <c r="D17">
+        <v>1</v>
+      </c>
+      <c r="E17">
         <v>1</v>
       </c>
     </row>
@@ -2464,10 +2562,13 @@
         <v>85</v>
       </c>
       <c r="C18" t="s">
-        <v>43</v>
+        <v>34</v>
       </c>
       <c r="D18">
         <v>4</v>
+      </c>
+      <c r="E18">
+        <v>0</v>
       </c>
     </row>
     <row r="20" spans="2:5" x14ac:dyDescent="0.25">
@@ -2475,19 +2576,583 @@
         <v>6</v>
       </c>
       <c r="D20">
-        <v>40</v>
+        <v>39</v>
+      </c>
+      <c r="E20">
+        <v>32</v>
       </c>
     </row>
     <row r="21" spans="2:5" x14ac:dyDescent="0.25">
       <c r="C21" s="1" t="s">
         <v>30</v>
       </c>
+      <c r="E21">
+        <v>121</v>
+      </c>
     </row>
     <row r="22" spans="2:5" x14ac:dyDescent="0.25">
       <c r="C22" s="1" t="s">
         <v>22</v>
       </c>
       <c r="E22">
+        <v>240</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="5">
+    <mergeCell ref="A1:F1"/>
+    <mergeCell ref="A2:F2"/>
+    <mergeCell ref="A3:F3"/>
+    <mergeCell ref="A4:F4"/>
+    <mergeCell ref="A5:F5"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:F21"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C17" sqref="C17"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="5.85546875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="70.85546875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="28.85546875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="10.42578125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="10.140625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="11.42578125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A1" s="9" t="s">
+        <v>109</v>
+      </c>
+      <c r="B1" s="9"/>
+      <c r="C1" s="9"/>
+      <c r="D1" s="9"/>
+      <c r="E1" s="9"/>
+      <c r="F1" s="9"/>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A2" s="6" t="s">
+        <v>38</v>
+      </c>
+      <c r="B2" s="6"/>
+      <c r="C2" s="6"/>
+      <c r="D2" s="6"/>
+      <c r="E2" s="6"/>
+      <c r="F2" s="6"/>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A3" s="8" t="s">
+        <v>114</v>
+      </c>
+      <c r="B3" s="8"/>
+      <c r="C3" s="8"/>
+      <c r="D3" s="8"/>
+      <c r="E3" s="8"/>
+      <c r="F3" s="8"/>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A4" s="6" t="s">
+        <v>7</v>
+      </c>
+      <c r="B4" s="6"/>
+      <c r="C4" s="6"/>
+      <c r="D4" s="6"/>
+      <c r="E4" s="6"/>
+      <c r="F4" s="6"/>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A5" s="10" t="s">
+        <v>115</v>
+      </c>
+      <c r="B5" s="10"/>
+      <c r="C5" s="10"/>
+      <c r="D5" s="10"/>
+      <c r="E5" s="10"/>
+      <c r="F5" s="10"/>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A7" s="2" t="s">
+        <v>58</v>
+      </c>
+      <c r="B7" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="C7" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="D7" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="E7" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="F7" s="2" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>113</v>
+      </c>
+      <c r="B8" t="s">
+        <v>112</v>
+      </c>
+      <c r="C8" t="s">
+        <v>23</v>
+      </c>
+      <c r="D8">
+        <v>1</v>
+      </c>
+      <c r="E8">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B9" t="s">
+        <v>106</v>
+      </c>
+      <c r="C9" t="s">
+        <v>23</v>
+      </c>
+      <c r="D9">
+        <v>1</v>
+      </c>
+      <c r="E9">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>87</v>
+      </c>
+      <c r="B10" t="s">
+        <v>107</v>
+      </c>
+      <c r="C10" t="s">
+        <v>43</v>
+      </c>
+      <c r="D10">
+        <v>8</v>
+      </c>
+      <c r="E10">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>99</v>
+      </c>
+      <c r="B11" t="s">
+        <v>93</v>
+      </c>
+      <c r="C11" t="s">
+        <v>23</v>
+      </c>
+      <c r="D11">
+        <v>5</v>
+      </c>
+      <c r="E11">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>100</v>
+      </c>
+      <c r="B12" t="s">
+        <v>94</v>
+      </c>
+      <c r="C12" t="s">
+        <v>23</v>
+      </c>
+      <c r="D12">
+        <v>4</v>
+      </c>
+      <c r="E12">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B13" t="s">
+        <v>111</v>
+      </c>
+      <c r="C13" t="s">
+        <v>23</v>
+      </c>
+      <c r="D13">
+        <v>1</v>
+      </c>
+      <c r="E13">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B14" t="s">
+        <v>85</v>
+      </c>
+      <c r="C14" t="s">
+        <v>23</v>
+      </c>
+      <c r="D14">
+        <v>6</v>
+      </c>
+      <c r="E14">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
+        <v>87</v>
+      </c>
+      <c r="B15" t="s">
+        <v>110</v>
+      </c>
+      <c r="C15" t="s">
+        <v>43</v>
+      </c>
+      <c r="D15">
+        <v>4</v>
+      </c>
+      <c r="E15">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
+        <v>87</v>
+      </c>
+      <c r="B16" s="5" t="s">
+        <v>126</v>
+      </c>
+      <c r="C16" t="s">
+        <v>43</v>
+      </c>
+      <c r="D16">
+        <v>3</v>
+      </c>
+      <c r="E16">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="17" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B17" t="s">
+        <v>108</v>
+      </c>
+      <c r="C17" t="s">
+        <v>23</v>
+      </c>
+      <c r="D17">
+        <v>1</v>
+      </c>
+      <c r="E17">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="19" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="C19" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="D19">
+        <v>34</v>
+      </c>
+      <c r="E19">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="20" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="C20" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="E20">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="21" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="C21" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="E21">
+        <v>240</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="5">
+    <mergeCell ref="A1:F1"/>
+    <mergeCell ref="A2:F2"/>
+    <mergeCell ref="A3:F3"/>
+    <mergeCell ref="A4:F4"/>
+    <mergeCell ref="A5:F5"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:F24"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D22" sqref="D22"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="5.85546875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="100.85546875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="28.85546875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="10.42578125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="10.140625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="11.42578125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A1" s="9" t="s">
+        <v>116</v>
+      </c>
+      <c r="B1" s="9"/>
+      <c r="C1" s="9"/>
+      <c r="D1" s="9"/>
+      <c r="E1" s="9"/>
+      <c r="F1" s="9"/>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A2" s="6" t="s">
+        <v>38</v>
+      </c>
+      <c r="B2" s="6"/>
+      <c r="C2" s="6"/>
+      <c r="D2" s="6"/>
+      <c r="E2" s="6"/>
+      <c r="F2" s="6"/>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A3" s="8" t="s">
+        <v>117</v>
+      </c>
+      <c r="B3" s="8"/>
+      <c r="C3" s="8"/>
+      <c r="D3" s="8"/>
+      <c r="E3" s="8"/>
+      <c r="F3" s="8"/>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A4" s="6" t="s">
+        <v>7</v>
+      </c>
+      <c r="B4" s="6"/>
+      <c r="C4" s="6"/>
+      <c r="D4" s="6"/>
+      <c r="E4" s="6"/>
+      <c r="F4" s="6"/>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A5" s="10" t="s">
+        <v>115</v>
+      </c>
+      <c r="B5" s="10"/>
+      <c r="C5" s="10"/>
+      <c r="D5" s="10"/>
+      <c r="E5" s="10"/>
+      <c r="F5" s="10"/>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A7" s="2" t="s">
+        <v>58</v>
+      </c>
+      <c r="B7" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="C7" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="D7" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="E7" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="F7" s="2" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B8" t="s">
+        <v>106</v>
+      </c>
+      <c r="C8" t="s">
+        <v>23</v>
+      </c>
+      <c r="D8">
+        <v>1</v>
+      </c>
+      <c r="E8">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B9" t="s">
+        <v>118</v>
+      </c>
+      <c r="C9" t="s">
+        <v>23</v>
+      </c>
+      <c r="D9">
+        <v>2</v>
+      </c>
+      <c r="E9">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B10" t="s">
+        <v>119</v>
+      </c>
+      <c r="C10" t="s">
+        <v>23</v>
+      </c>
+      <c r="D10">
+        <v>1</v>
+      </c>
+      <c r="E10">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B11" t="s">
+        <v>120</v>
+      </c>
+      <c r="C11" t="s">
+        <v>34</v>
+      </c>
+      <c r="D11">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B12" t="s">
+        <v>121</v>
+      </c>
+      <c r="C12" t="s">
+        <v>23</v>
+      </c>
+      <c r="D12">
+        <v>1</v>
+      </c>
+      <c r="E12">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B13" t="s">
+        <v>123</v>
+      </c>
+      <c r="C13" t="s">
+        <v>34</v>
+      </c>
+      <c r="D13">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B14" t="s">
+        <v>124</v>
+      </c>
+      <c r="C14" t="s">
+        <v>23</v>
+      </c>
+      <c r="D14">
+        <v>2</v>
+      </c>
+      <c r="E14">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B15" t="s">
+        <v>125</v>
+      </c>
+      <c r="C15" t="s">
+        <v>34</v>
+      </c>
+      <c r="D15">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B16" t="s">
+        <v>110</v>
+      </c>
+      <c r="C16" t="s">
+        <v>43</v>
+      </c>
+      <c r="D16">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="17" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B17" t="s">
+        <v>127</v>
+      </c>
+      <c r="C17" t="s">
+        <v>34</v>
+      </c>
+      <c r="D17">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="18" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B18" t="s">
+        <v>128</v>
+      </c>
+      <c r="C18" t="s">
+        <v>34</v>
+      </c>
+      <c r="D18">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="19" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B19" t="s">
+        <v>85</v>
+      </c>
+      <c r="D19">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="20" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B20" t="s">
+        <v>122</v>
+      </c>
+      <c r="D20">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="22" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="C22" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="D22">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="23" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="C23" s="1" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="24" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="C24" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="E24">
         <v>240</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Lagt till powerpointen till presentationen
Även uppdaterat Iterationsplanen
</commit_message>
<xml_diff>
--- a/Iterationsplan_as223jx.xlsx
+++ b/Iterationsplan_as223jx.xlsx
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="333" uniqueCount="130">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="335" uniqueCount="131">
   <si>
     <t>Tidsrapport v 14</t>
   </si>
@@ -411,6 +411,9 @@
   </si>
   <si>
     <t>Hantera "Upp"-knappen i headern</t>
+  </si>
+  <si>
+    <t>Gör powerpointpresentationen</t>
   </si>
 </sst>
 </file>
@@ -1437,7 +1440,7 @@
   <dimension ref="A1:F20"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="F14" sqref="F14"/>
+      <selection activeCell="B32" sqref="B32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2618,7 +2621,7 @@
   <dimension ref="A1:F21"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C17" sqref="C17"/>
+      <selection activeCell="C31" sqref="C31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2900,10 +2903,10 @@
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F26"/>
+  <dimension ref="A1:F27"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D24" sqref="D24"/>
+      <selection activeCell="D21" sqref="D21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3153,10 +3156,13 @@
         <v>128</v>
       </c>
       <c r="C20" t="s">
-        <v>34</v>
+        <v>43</v>
       </c>
       <c r="D20">
         <v>5</v>
+      </c>
+      <c r="E20">
+        <v>4</v>
       </c>
     </row>
     <row r="21" spans="2:5" x14ac:dyDescent="0.25">
@@ -3184,24 +3190,38 @@
         <v>1</v>
       </c>
     </row>
-    <row r="24" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="C24" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="D24">
-        <v>38</v>
+    <row r="23" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B23" t="s">
+        <v>130</v>
+      </c>
+      <c r="C23" t="s">
+        <v>43</v>
+      </c>
+      <c r="E23">
+        <v>7</v>
       </c>
     </row>
     <row r="25" spans="2:5" x14ac:dyDescent="0.25">
       <c r="C25" s="1" t="s">
-        <v>30</v>
+        <v>6</v>
+      </c>
+      <c r="D25">
+        <v>38</v>
+      </c>
+      <c r="E25">
+        <v>34</v>
       </c>
     </row>
     <row r="26" spans="2:5" x14ac:dyDescent="0.25">
       <c r="C26" s="1" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="27" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="C27" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="E26">
+      <c r="E27">
         <v>240</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Uppdaterat med senaste versionen av appen
</commit_message>
<xml_diff>
--- a/Iterationsplan_as223jx.xlsx
+++ b/Iterationsplan_as223jx.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9302"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="480" yWindow="30" windowWidth="22995" windowHeight="10050" activeTab="7"/>
+    <workbookView xWindow="480" yWindow="30" windowWidth="22995" windowHeight="10050" firstSheet="1" activeTab="8"/>
   </bookViews>
   <sheets>
     <sheet name="Iteration 0" sheetId="1" r:id="rId1"/>
@@ -14,14 +14,15 @@
     <sheet name="Iteration 4" sheetId="5" r:id="rId5"/>
     <sheet name="Iteration 5" sheetId="6" r:id="rId6"/>
     <sheet name="Iteration 6" sheetId="7" r:id="rId7"/>
-    <sheet name="Sheet2" sheetId="8" r:id="rId8"/>
+    <sheet name="Iteration 7" sheetId="8" r:id="rId8"/>
+    <sheet name="Iteration 8" sheetId="9" r:id="rId9"/>
   </sheets>
   <calcPr calcId="144525"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="335" uniqueCount="131">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="373" uniqueCount="145">
   <si>
     <t>Tidsrapport v 14</t>
   </si>
@@ -389,9 +390,6 @@
     <t>Fixa att om man ändrar namn i Redigera Recept ska den gamla filen tas bort och en ny sparas med nya namnet.</t>
   </si>
   <si>
-    <t>Skapa Iterationsplan för Iteration 8</t>
-  </si>
-  <si>
     <t>Fixa så nya receptradernas "Antal"-textfält har siffror som standardinmatning.</t>
   </si>
   <si>
@@ -414,6 +412,51 @@
   </si>
   <si>
     <t>Gör powerpointpresentationen</t>
+  </si>
+  <si>
+    <t>Iterationsplan Iteration 8</t>
+  </si>
+  <si>
+    <t>Lyckats fixa allt med mina spinner/dropdown-fält, och alla grundfuktioner fungerar nästan helt som de ska. Börjat lite med att lägga in färger och fixa gränssnittet.</t>
+  </si>
+  <si>
+    <t>Målet med denna iteration är att bli färdig med alla slutinlämingar, redovisningar etc.</t>
+  </si>
+  <si>
+    <t>Presentation av applikationen</t>
+  </si>
+  <si>
+    <t>Skriva sammanfattning från Workshop III</t>
+  </si>
+  <si>
+    <t>Post Mortem</t>
+  </si>
+  <si>
+    <t>Ladda upp Projektmappen och .apk-filen till reprot, samt testa om .apk-filen funkar</t>
+  </si>
+  <si>
+    <t>Fyll i formuläter för slutleverans och självvärdering</t>
+  </si>
+  <si>
+    <t>Fixa så man kan lämna en tom ingrediensrad</t>
+  </si>
+  <si>
+    <t>Fixa så designen i "Redigera recept" matchar designen i "Nytt recept"</t>
+  </si>
+  <si>
+    <t>Ladda upp videodemostrationen</t>
+  </si>
+  <si>
+    <t>Gör klart sidan för slutuppgiften i Gränssnittsutveckling</t>
+  </si>
+  <si>
+    <t>Spela in videodemonstration</t>
+  </si>
+  <si>
+    <t>Fixa grundläggande färger i appens startsida samt "Visa recept"-sidan</t>
+  </si>
+  <si>
+    <t>Skapa en bekräftelseruta innan ett recept raderas</t>
   </si>
 </sst>
 </file>
@@ -2836,7 +2879,7 @@
         <v>87</v>
       </c>
       <c r="B16" s="5" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="C16" t="s">
         <v>43</v>
@@ -2903,10 +2946,10 @@
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F27"/>
+  <dimension ref="A1:F26"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D21" sqref="D21"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="F26" sqref="A1:F26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3061,7 +3104,7 @@
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B13" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="C13" t="s">
         <v>23</v>
@@ -3070,7 +3113,7 @@
         <v>2</v>
       </c>
       <c r="E13">
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.25">
@@ -3089,7 +3132,7 @@
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B15" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="C15" t="s">
         <v>23</v>
@@ -3103,7 +3146,7 @@
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B16" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="C16" t="s">
         <v>23</v>
@@ -3117,13 +3160,16 @@
     </row>
     <row r="17" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B17" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="C17" t="s">
         <v>34</v>
       </c>
       <c r="D17">
         <v>4</v>
+      </c>
+      <c r="E17">
+        <v>0</v>
       </c>
     </row>
     <row r="18" spans="2:5" x14ac:dyDescent="0.25">
@@ -3142,7 +3188,7 @@
     </row>
     <row r="19" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B19" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="C19" t="s">
         <v>34</v>
@@ -3150,10 +3196,13 @@
       <c r="D19">
         <v>1</v>
       </c>
+      <c r="E19">
+        <v>0</v>
+      </c>
     </row>
     <row r="20" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B20" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="C20" t="s">
         <v>43</v>
@@ -3162,7 +3211,7 @@
         <v>5</v>
       </c>
       <c r="E20">
-        <v>4</v>
+        <v>6</v>
       </c>
     </row>
     <row r="21" spans="2:5" x14ac:dyDescent="0.25">
@@ -3181,47 +3230,330 @@
     </row>
     <row r="22" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B22" t="s">
-        <v>122</v>
+        <v>129</v>
       </c>
       <c r="C22" t="s">
-        <v>34</v>
-      </c>
-      <c r="D22">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="23" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B23" t="s">
-        <v>130</v>
-      </c>
-      <c r="C23" t="s">
-        <v>43</v>
-      </c>
-      <c r="E23">
-        <v>7</v>
+        <v>23</v>
+      </c>
+      <c r="E22">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="24" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="C24" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="D24">
+        <v>38</v>
+      </c>
+      <c r="E24">
+        <v>38</v>
       </c>
     </row>
     <row r="25" spans="2:5" x14ac:dyDescent="0.25">
       <c r="C25" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="D25">
-        <v>38</v>
+        <v>30</v>
       </c>
       <c r="E25">
-        <v>34</v>
+        <v>51</v>
       </c>
     </row>
     <row r="26" spans="2:5" x14ac:dyDescent="0.25">
       <c r="C26" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="E26">
+        <v>240</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="5">
+    <mergeCell ref="A1:F1"/>
+    <mergeCell ref="A2:F2"/>
+    <mergeCell ref="A3:F3"/>
+    <mergeCell ref="A4:F4"/>
+    <mergeCell ref="A5:F5"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:F24"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B14" sqref="B14"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="4.85546875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="100.85546875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="28.85546875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="10.42578125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="10.140625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="11.42578125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A1" s="9" t="s">
+        <v>130</v>
+      </c>
+      <c r="B1" s="9"/>
+      <c r="C1" s="9"/>
+      <c r="D1" s="9"/>
+      <c r="E1" s="9"/>
+      <c r="F1" s="9"/>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A2" s="6" t="s">
+        <v>38</v>
+      </c>
+      <c r="B2" s="6"/>
+      <c r="C2" s="6"/>
+      <c r="D2" s="6"/>
+      <c r="E2" s="6"/>
+      <c r="F2" s="6"/>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A3" s="8" t="s">
+        <v>131</v>
+      </c>
+      <c r="B3" s="8"/>
+      <c r="C3" s="8"/>
+      <c r="D3" s="8"/>
+      <c r="E3" s="8"/>
+      <c r="F3" s="8"/>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A4" s="6" t="s">
+        <v>7</v>
+      </c>
+      <c r="B4" s="6"/>
+      <c r="C4" s="6"/>
+      <c r="D4" s="6"/>
+      <c r="E4" s="6"/>
+      <c r="F4" s="6"/>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A5" s="10" t="s">
+        <v>132</v>
+      </c>
+      <c r="B5" s="10"/>
+      <c r="C5" s="10"/>
+      <c r="D5" s="10"/>
+      <c r="E5" s="10"/>
+      <c r="F5" s="10"/>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A7" s="2" t="s">
+        <v>58</v>
+      </c>
+      <c r="B7" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="C7" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="D7" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="E7" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="F7" s="2" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B8" t="s">
+        <v>133</v>
+      </c>
+      <c r="C8" t="s">
+        <v>23</v>
+      </c>
+      <c r="D8">
+        <v>2</v>
+      </c>
+      <c r="E8">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B9" t="s">
+        <v>134</v>
+      </c>
+      <c r="C9" t="s">
+        <v>23</v>
+      </c>
+      <c r="D9">
+        <v>1</v>
+      </c>
+      <c r="E9">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B10" t="s">
+        <v>138</v>
+      </c>
+      <c r="C10" t="s">
+        <v>43</v>
+      </c>
+      <c r="D10">
+        <v>2</v>
+      </c>
+      <c r="E10">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B11" t="s">
+        <v>139</v>
+      </c>
+      <c r="C11" t="s">
+        <v>23</v>
+      </c>
+      <c r="D11">
+        <v>2</v>
+      </c>
+      <c r="E11">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B12" t="s">
+        <v>143</v>
+      </c>
+      <c r="C12" t="s">
+        <v>23</v>
+      </c>
+      <c r="D12">
+        <v>3</v>
+      </c>
+      <c r="E12">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B13" t="s">
+        <v>144</v>
+      </c>
+      <c r="C13" t="s">
+        <v>23</v>
+      </c>
+      <c r="D13">
+        <v>1</v>
+      </c>
+      <c r="E13">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B14" t="s">
+        <v>142</v>
+      </c>
+      <c r="C14" t="s">
+        <v>34</v>
+      </c>
+      <c r="D14">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B15" t="s">
+        <v>140</v>
+      </c>
+      <c r="C15" t="s">
+        <v>34</v>
+      </c>
+      <c r="D15">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B16" t="s">
+        <v>136</v>
+      </c>
+      <c r="C16" t="s">
+        <v>43</v>
+      </c>
+      <c r="D16">
+        <v>1</v>
+      </c>
+      <c r="E16">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="17" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B17" t="s">
+        <v>141</v>
+      </c>
+      <c r="C17" t="s">
+        <v>43</v>
+      </c>
+      <c r="D17">
+        <v>5</v>
+      </c>
+      <c r="E17">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="18" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B18" t="s">
+        <v>85</v>
+      </c>
+      <c r="C18" t="s">
+        <v>34</v>
+      </c>
+      <c r="D18">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="19" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B19" t="s">
+        <v>135</v>
+      </c>
+      <c r="C19" t="s">
+        <v>43</v>
+      </c>
+      <c r="D19">
+        <v>3</v>
+      </c>
+      <c r="E19">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="20" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B20" t="s">
+        <v>137</v>
+      </c>
+      <c r="C20" t="s">
+        <v>34</v>
+      </c>
+      <c r="D20">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="22" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="C22" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="D22">
         <v>30</v>
       </c>
     </row>
-    <row r="27" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="C27" s="1" t="s">
+    <row r="23" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="C23" s="1" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="24" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="C24" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="E27">
+      <c r="E24">
         <v>240</v>
       </c>
     </row>

</xml_diff>